<commit_message>
test cases added and new file sample
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/target/test-classes/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/target/test-classes/TestData/OETestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19989D3-7526-41C4-BA74-D144F48421ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6036AB9F-87EC-456C-A7F9-786B393245D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
@@ -1193,11 +1193,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A830C6A-2351-42AD-9726-C7D67A089D6F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -1297,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEDDC4C-1822-423E-A6B2-E3DFEA3895E6}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>